<commit_message>
Switch to ollama AI
</commit_message>
<xml_diff>
--- a/AI配置.xlsx
+++ b/AI配置.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\KnoLib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4428927C-2875-45CE-828E-B75CBBBE9154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA45003C-3445-4D9F-A848-4A842368527A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="配置" sheetId="1" r:id="rId1"/>
@@ -51,15 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
-  <si>
-    <t>API Key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>生成内容概括</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Y</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -89,27 +81,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>投票和打分</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>输出API计价信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>生成章节总结并嵌入正文</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>表情符号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>N</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>xxxxxxxxxxx</t>
+    <t>Ollama Host</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ollama Port</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ollama Model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.96.246</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>投票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wangshenzhi/llama3-8b-chinese-chat-ollama-q8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -452,81 +448,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="27.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>11434</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="B6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -534,38 +523,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02000C99-72CF-4549-9323-1E31A1D9E2E1}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.125" customWidth="1"/>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="22.1328125" customWidth="1"/>
+    <col min="2" max="2" width="20.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
       <c r="B2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AI model changes to Deepseek
</commit_message>
<xml_diff>
--- a/AI配置.xlsx
+++ b/AI配置.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\KnoLib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA45003C-3445-4D9F-A848-4A842368527A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F598B5BF-6E52-49DD-BDB7-985930623DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21630" windowHeight="10515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="配置" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Y</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -97,15 +97,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>192.168.96.246</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>投票</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>wangshenzhi/llama3-8b-chinese-chat-ollama-q8</t>
+    <t>deepseek-r1:14b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示语义分析打分及内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>127.0.0.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -448,23 +452,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.46484375" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -472,15 +476,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -488,15 +492,15 @@
         <v>11434</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -504,11 +508,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>0</v>
       </c>
     </row>
@@ -523,17 +535,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02000C99-72CF-4549-9323-1E31A1D9E2E1}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1328125" customWidth="1"/>
-    <col min="2" max="2" width="20.46484375" customWidth="1"/>
+    <col min="1" max="1" width="22.125" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -541,7 +553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -549,9 +561,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>8</v>

</xml_diff>